<commit_message>
fixed case with old steelmaking routes. paths.yml deleted, and paths to be changed manually
</commit_message>
<xml_diff>
--- a/support/inventories/steelmakingroutes.xlsx
+++ b/support/inventories/steelmakingroutes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365.sharepoint.com/sites/DENG-SESAM/Documenti condivisi/c-Research/a-Datasets/IAM COMPACT Study 9/Inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/ExioSteel/support/inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{2198A223-5109-7D4A-AC0F-C03BB1A2A880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8266F7BE-040E-3B43-AC40-C294580A57C5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5175C8FA-9193-2546-B7B0-CA766D1EF3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1720" yWindow="-21680" windowWidth="30240" windowHeight="17480" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3035" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3041" uniqueCount="811">
   <si>
     <t>Region</t>
   </si>
@@ -2466,15 +2466,6 @@
   </si>
   <si>
     <t>Percentage</t>
-  </si>
-  <si>
-    <t>Electricity, fossil</t>
-  </si>
-  <si>
-    <t>Electricity, nuclear</t>
-  </si>
-  <si>
-    <t>Electricity, renewable</t>
   </si>
 </sst>
 </file>
@@ -3213,10 +3204,21 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H4"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -3333,10 +3335,21 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H4"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -3453,10 +3466,21 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H27"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -4171,10 +4195,21 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -12041,15 +12076,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AC2EE9-9F08-5249-96FF-38A0DFD800C4}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -12059,17 +12094,47 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>811</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>812</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>813</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -12699,17 +12764,20 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -12855,10 +12923,21 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H8"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -13080,13 +13159,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -13301,10 +13388,21 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H4"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -13423,10 +13521,21 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -14140,10 +14249,21 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H5"/>
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -14281,6 +14401,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e">
@@ -14289,15 +14418,6 @@
     <TaxCatchAll xmlns="e67e9a88-35e1-4b39-8da9-a609eb308282" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14556,6 +14676,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C8DC52B-6AB8-415F-A696-2702D71CB2DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5876A66E-0E66-487B-A9B1-3338B55445E2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
@@ -14572,14 +14700,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C8DC52B-6AB8-415F-A696-2702D71CB2DA}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E69E6D-8D8C-483F-B9A9-F0826C8E294C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
+    <ds:schemaRef ds:uri="e67e9a88-35e1-4b39-8da9-a609eb308282"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E69E6D-8D8C-483F-B9A9-F0826C8E294C}"/>
 </file>
</xml_diff>